<commit_message>
Added a warning when not all analytes from the analyte list are present in the data
</commit_message>
<xml_diff>
--- a/inst/extdata/Analyte_list.xlsx
+++ b/inst/extdata/Analyte_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slsiekman\Documents\glycodash\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B1ADD2-D046-41B7-99F4-B833CAD0329B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A5CE8EE-3FD6-4366-989E-A974393F449D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{CC0A665E-DF79-417A-AA6B-1CB1B1BDCFDD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Analyte</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>IgGI1H4N4S1</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -451,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB8924D0-A2C1-4371-B364-C88A5C9F39A7}">
-  <dimension ref="A1:A15"/>
+  <dimension ref="A1:A16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,6 +538,11 @@
     <row r="15" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed confidential data and updated tests.
</commit_message>
<xml_diff>
--- a/inst/extdata/Analyte_list.xlsx
+++ b/inst/extdata/Analyte_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slsiekman\Documents\glycodash\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A5CE8EE-3FD6-4366-989E-A974393F449D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D5F68ED-485C-43B7-BBDC-9FF4694E42C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{CC0A665E-DF79-417A-AA6B-1CB1B1BDCFDD}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{CC0A665E-DF79-417A-AA6B-1CB1B1BDCFDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Analyte</t>
   </si>
@@ -78,12 +78,6 @@
   </si>
   <si>
     <t>IgGI1H5N5F1S1</t>
-  </si>
-  <si>
-    <t>IgGI1H4N4S1</t>
-  </si>
-  <si>
-    <t>test</t>
   </si>
 </sst>
 </file>
@@ -454,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB8924D0-A2C1-4371-B364-C88A5C9F39A7}">
-  <dimension ref="A1:A16"/>
+  <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,43 +501,36 @@
     </row>
     <row r="9" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="A15" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add column name "analyte"
</commit_message>
<xml_diff>
--- a/inst/extdata/Analyte_list.xlsx
+++ b/inst/extdata/Analyte_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slsiekman\Documents\glycodash\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D5F68ED-485C-43B7-BBDC-9FF4694E42C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6722D47-E9D2-4FB3-9A9E-167BBB0DBC0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{CC0A665E-DF79-417A-AA6B-1CB1B1BDCFDD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{CC0A665E-DF79-417A-AA6B-1CB1B1BDCFDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
-    <t>Analyte</t>
-  </si>
-  <si>
     <t>IgGI1H3N4</t>
   </si>
   <si>
@@ -78,6 +75,9 @@
   </si>
   <si>
     <t>IgGI1H5N5F1S1</t>
+  </si>
+  <si>
+    <t>analyte</t>
   </si>
 </sst>
 </file>
@@ -451,7 +451,7 @@
   <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,72 +461,72 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>